<commit_message>
few more error handling 31 July 2023
</commit_message>
<xml_diff>
--- a/LOGS/ed568ca4-0c35-40f7-b53d-a29d16d0bc1d/main_page_service_output/main_pages.xlsx
+++ b/LOGS/ed568ca4-0c35-40f7-b53d-a29d16d0bc1d/main_page_service_output/main_pages.xlsx
@@ -8,8 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="cbs_8" sheetId="1" r:id="rId1"/>
-    <sheet name="cpl_5" sheetId="2" r:id="rId2"/>
-    <sheet name="ccf_9" sheetId="3" r:id="rId3"/>
+    <sheet name="cpl_7" sheetId="2" r:id="rId2"/>
+    <sheet name="cpl_5" sheetId="3" r:id="rId3"/>
+    <sheet name="ccf_9" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -1571,6 +1572,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1955,7 +1968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F27"/>
   <sheetViews>

</xml_diff>